<commit_message>
1.3.1 tratamento com python(pandas)
</commit_message>
<xml_diff>
--- a/dados_realiz-2024_tratados.xlsx
+++ b/dados_realiz-2024_tratados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e62e7c97e835051/Altieri/Softwares/Dev/Projetos Pessoais/Projeto_Carteira_Investimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_064DF1ACD3E0D00C0FFA3711595ED87656CDF7CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{044440D2-F05E-41B7-A44A-027AD5F7AAC7}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_3B6D53B9D3905E58E7FA2611595ED87656CD67C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C433B75B-91A8-4DE0-8917-D73C5641D211}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20280" yWindow="-1980" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I19"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +592,7 @@
         <v>898.16</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -607,10 +607,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>527</v>
+        <v>552</v>
       </c>
       <c r="O2">
-        <v>6323.97</v>
+        <v>6623.97</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>706.16</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -654,10 +654,10 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>286.82</v>
+        <v>311.82</v>
       </c>
       <c r="O3">
-        <v>3441.83</v>
+        <v>3741.83</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -936,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>112.55</v>
+        <v>137.55000000000001</v>
       </c>
       <c r="O9">
-        <v>1350.62</v>
+        <v>1650.62</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>